<commit_message>
GS-13.1 - Estrutura frontend
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Zago\Desktop\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCB186C-5693-44E4-9E71-6734A8F26913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CDC67C-67FE-4AA1-8B41-2855A8D9D68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>User storys</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Definir nome para o aplicativo</t>
+  </si>
+  <si>
+    <t>13.1</t>
   </si>
 </sst>
 </file>
@@ -623,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,49 +916,49 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="6"/>
       <c r="C33" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="6"/>
       <c r="C34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="6"/>
       <c r="C35" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="6"/>
       <c r="C36" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="6"/>
       <c r="C37" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="6"/>
       <c r="C38" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>13</v>
       </c>
@@ -965,22 +968,25 @@
       <c r="C39" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="6"/>
       <c r="C40" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5" t="s">
@@ -989,16 +995,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="A30:A38"/>
@@ -1011,6 +1007,16 @@
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B30:B38"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-12.1 - Diagrama entidade relacionamento
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Zago\Desktop\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CDC67C-67FE-4AA1-8B41-2855A8D9D68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC7F0EE-CE7B-4B33-88FD-F1F1A3C81FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +954,7 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -965,7 +965,7 @@
       <c r="B39" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -995,6 +995,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="A30:A38"/>
@@ -1007,16 +1017,6 @@
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B30:B38"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-2.1 - Implementado rotina para cadastro, atualização, exclusão e listagem do treino no backend
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Zago\Desktop\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC7F0EE-CE7B-4B33-88FD-F1F1A3C81FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB22F7F-7E5C-47A6-9030-74625B47817B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>User storys</t>
   </si>
@@ -102,12 +102,6 @@
     <t>Criar tela com os exercicios e que permita alterar a quantidade de reps, cargas e series durante o treino</t>
   </si>
   <si>
-    <t>Criação da rotina para cadastro, atualização, exclusão do treino no próprio aparelho</t>
-  </si>
-  <si>
-    <t>Popular a tabela de exercicios no próprio aparelho para permitir a edição offline</t>
-  </si>
-  <si>
     <t>Criação de rotina para retornar todos os treinos do usuário</t>
   </si>
   <si>
@@ -220,6 +214,39 @@
   </si>
   <si>
     <t>13.1</t>
+  </si>
+  <si>
+    <t>Fazer a conexão do backend com o banco de dados</t>
+  </si>
+  <si>
+    <t>Criar as tabelas referentes ao treino individual no banco de dados</t>
+  </si>
+  <si>
+    <t>Popular a tabela de exercicios no próprio aparelho para permitir a edição offline, fazendo um endpoint que retorne todos os exercicios cadastrados no banco de dados</t>
+  </si>
+  <si>
+    <t>Criação da rotina para cadastro, atualização, exclusão e listagem do treino no backend</t>
+  </si>
+  <si>
+    <t>Criação da rotina para cadastro, atualização, exclusão e listagem do treino no aparelho</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.6</t>
   </si>
 </sst>
 </file>
@@ -243,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +280,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -290,6 +323,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -626,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,9 +685,9 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -651,274 +696,292 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="6"/>
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="D5" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>4</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="6"/>
       <c r="C18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="7">
+        <v>6</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>7</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>35</v>
-      </c>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="6"/>
       <c r="C22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
-        <v>8</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>6</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="6"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>7</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="6"/>
       <c r="C25" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>9</v>
-      </c>
-      <c r="B26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <v>8</v>
       </c>
+      <c r="B26" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
-        <v>10</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="6"/>
       <c r="C28" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="6"/>
       <c r="C31" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="6"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="6"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>12</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>41</v>
       </c>
@@ -930,93 +993,114 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="6"/>
       <c r="C35" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="6"/>
       <c r="C36" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="6"/>
       <c r="C37" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
-        <v>13</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="5" t="s">
-        <v>56</v>
+      <c r="C40" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="6"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>13</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="C42" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="5" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B33:B41"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A5:A9"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B5:B10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-2.7 - backup banco de dados + postman
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Zago\Desktop\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB22F7F-7E5C-47A6-9030-74625B47817B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2172B111-92FC-4F0E-99EC-8D71ED20B1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>User storys</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>2.6</t>
+  </si>
+  <si>
+    <t>Criar tela de login</t>
+  </si>
+  <si>
+    <t>2.7</t>
   </si>
 </sst>
 </file>
@@ -671,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,332 +781,342 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>3</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>4</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+    <row r="18" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>6</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="6"/>
       <c r="C22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="6"/>
       <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>7</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>8</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="6"/>
       <c r="C28" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>9</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+    <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>10</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
         <v>11</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+    <row r="34" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <v>12</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="6"/>
       <c r="C35" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="6"/>
       <c r="C36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="6"/>
       <c r="C37" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="6"/>
       <c r="C38" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="6"/>
       <c r="C39" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="6"/>
       <c r="C40" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+    <row r="43" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>13</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="6"/>
       <c r="C44" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="6"/>
       <c r="C45" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="5" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A33:A41"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B33:B41"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A34:A42"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B34:B42"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B5:B11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-4.1 - Rotina para atualizar as cargas e repetições do treino padrão ao finalizar um treino
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Zago\Desktop\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2172B111-92FC-4F0E-99EC-8D71ED20B1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4EA361-FD29-47C7-B8EE-2C3631C8B34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>User storys</t>
   </si>
@@ -45,9 +45,6 @@
     <t>DOR</t>
   </si>
   <si>
-    <t>Eu como usuário quero poder criar mais de um treino</t>
-  </si>
-  <si>
     <t>Eu como usuário quero marcar minhas cargas nos exercicios a cada treino</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Criação do endpoint para cadastro, atualização, exclusão do treino</t>
   </si>
   <si>
-    <t>Design da tela para listar os treinos</t>
-  </si>
-  <si>
     <t>Implementação do login no backend  com usuário ou email e senha</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>Criar tela com os exercicios e que permita alterar a quantidade de reps, cargas e series durante o treino</t>
   </si>
   <si>
-    <t>Criação de rotina para retornar todos os treinos do usuário</t>
-  </si>
-  <si>
     <t>Criar rotina com os exercicios e que permita alterar a quantidade de reps, cargas e series durante o treino</t>
   </si>
   <si>
@@ -114,9 +105,6 @@
     <t>Eu como usuário quero poder montar meu treino offline com exercicios, séries, técnicas avançadas e número de repetições personalizadas</t>
   </si>
   <si>
-    <t>Criação da tela que lista os treinos do usuário offline</t>
-  </si>
-  <si>
     <t>Criar tela listando todos os treinos feitos com histórico de cargas e exercicios</t>
   </si>
   <si>
@@ -253,6 +241,12 @@
   </si>
   <si>
     <t>2.7</t>
+  </si>
+  <si>
+    <t>Criar rotina no aparelho para ao finalizar o treino, o usuário tenha a opção de atualizar as cargas e repetições, e tornar padrão naquele treino</t>
+  </si>
+  <si>
+    <t>4.1</t>
   </si>
 </sst>
 </file>
@@ -308,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -328,6 +322,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -336,12 +339,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +690,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -703,420 +700,405 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>5</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>2</v>
-      </c>
-      <c r="B5" s="9" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="10" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>6</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>7</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>8</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>10</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
         <v>12</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>4</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>5</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>6</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>7</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
-        <v>8</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>9</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
-        <v>10</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="1" t="s">
+    <row r="37" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>13</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="1" t="s">
+      <c r="C41" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>11</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="D41" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
-        <v>12</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
-        <v>13</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>52</v>
-      </c>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="9"/>
       <c r="C43" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="6"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A34:A42"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B34:B42"/>
+  <mergeCells count="20">
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B5:B11"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A32:A40"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B32:B40"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1137,22 +1119,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GS-1.1 - Tela de login adaptada
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Zago\Desktop\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4EA361-FD29-47C7-B8EE-2C3631C8B34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CD573E-9AFB-4662-94C8-D09E9A398797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
   <si>
     <t>User storys</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Design da tela de login e cadastro</t>
   </si>
   <si>
-    <t>Criação das telas de login e cadastro e integração com o backend</t>
-  </si>
-  <si>
     <t>Design da tela com os exercicios do treino iniciado no dia</t>
   </si>
   <si>
@@ -247,6 +244,24 @@
   </si>
   <si>
     <t>4.1</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Criação da tela de cadastro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criação das telas de login </t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Testes com o dispositivo offline</t>
+  </si>
+  <si>
+    <t>4.2</t>
   </si>
 </sst>
 </file>
@@ -302,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,25 +334,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -674,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +711,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -700,405 +721,439 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>2</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>4</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>5</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>6</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>7</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>8</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>10</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>4</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>5</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>6</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>7</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="B34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>12</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="1" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>9</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
-        <v>10</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>11</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
-        <v>12</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="1" t="s">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="1" t="s">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="5" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
+        <v>13</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
-        <v>13</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="5" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="5" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A32:A40"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B32:B40"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A35:A43"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B35:B43"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-1.2 - Tela de cadastro + Exception Middleware
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Zago\Desktop\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CD573E-9AFB-4662-94C8-D09E9A398797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C2719B-68EC-4BE9-BC9A-96257794C648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -340,6 +340,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -347,18 +350,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -698,7 +692,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,10 +715,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -732,49 +726,49 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
@@ -783,8 +777,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="6" t="s">
         <v>56</v>
       </c>
@@ -793,8 +787,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="5" t="s">
         <v>55</v>
       </c>
@@ -803,8 +797,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="5" t="s">
         <v>54</v>
       </c>
@@ -813,8 +807,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="5" t="s">
         <v>57</v>
       </c>
@@ -823,8 +817,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="5" t="s">
         <v>65</v>
       </c>
@@ -833,8 +827,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="5" t="s">
         <v>58</v>
       </c>
@@ -843,10 +837,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="9">
         <v>4</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -855,25 +849,25 @@
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="9" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="8" t="s">
         <v>67</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -881,20 +875,20 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="9">
         <v>5</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -902,24 +896,24 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -927,31 +921,31 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="9">
         <v>7</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -959,17 +953,17 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="9">
         <v>8</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -977,15 +971,15 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1002,10 +996,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="9">
         <v>10</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1013,8 +1007,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="7"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="1" t="s">
         <v>44</v>
       </c>
@@ -1031,10 +1025,10 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="9">
         <v>12</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1042,57 +1036,57 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="5" t="s">
         <v>51</v>
       </c>
@@ -1134,6 +1128,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="B14:B18"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="A44:A47"/>
@@ -1149,11 +1148,6 @@
     <mergeCell ref="B35:B43"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="A6:A13"/>
-    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Adaptando para sqlite os dados armazenados no dispositivo
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Zago\Desktop\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C2719B-68EC-4BE9-BC9A-96257794C648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF296BD8-9895-419B-B201-78C7FE758CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -692,7 +692,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,10 +759,10 @@
       <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="6" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GS-4.2 - Testes, conclusão de treinos offline
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Zago\Desktop\Projetos\AppTreinos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF296BD8-9895-419B-B201-78C7FE758CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C97993-FE3F-423B-8316-0B7EBB418A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>User storys</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>4.2</t>
+  </si>
+  <si>
+    <t>Inserir rotina para sincronizar no banco de dados os treinos finalizados não sincronizados</t>
+  </si>
+  <si>
+    <t>4.3</t>
   </si>
 </sst>
 </file>
@@ -337,20 +343,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -689,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,10 +721,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -726,15 +732,15 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="5" t="s">
         <v>71</v>
       </c>
@@ -743,8 +749,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="5" t="s">
         <v>70</v>
       </c>
@@ -753,22 +759,22 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="10">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
@@ -777,8 +783,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="6" t="s">
         <v>56</v>
       </c>
@@ -787,8 +793,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="5" t="s">
         <v>55</v>
       </c>
@@ -797,8 +803,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="5" t="s">
         <v>54</v>
       </c>
@@ -807,8 +813,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="5" t="s">
         <v>57</v>
       </c>
@@ -817,8 +823,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="5" t="s">
         <v>65</v>
       </c>
@@ -827,8 +833,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="5" t="s">
         <v>58</v>
       </c>
@@ -837,10 +843,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="10">
         <v>4</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -849,25 +855,25 @@
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="8" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -875,279 +881,289 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="7" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+    <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
         <v>5</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B20" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+    <row r="21" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
       <c r="B21" s="12"/>
       <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
         <v>6</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="12"/>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="12"/>
       <c r="C25" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+    <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
         <v>7</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B27" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
         <v>8</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B29" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="12"/>
       <c r="C30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>9</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
         <v>10</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B33" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="1" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>11</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+    <row r="36" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
         <v>12</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B36" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="12"/>
       <c r="C37" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="12"/>
       <c r="C38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="12"/>
       <c r="C39" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
       <c r="B40" s="12"/>
       <c r="C40" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
       <c r="B41" s="12"/>
       <c r="C41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="12"/>
       <c r="C42" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="5" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
+    <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
         <v>13</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B45" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="5" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="5" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="5" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="5" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A36:A44"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B36:B44"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="A6:A13"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A35:A43"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B35:B43"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-5.1 - Tela principal + drawer com navegação entre telas
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C97993-FE3F-423B-8316-0B7EBB418A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E1D15-0586-414E-A874-6DD1D9FA5C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
   <si>
     <t>User storys</t>
   </si>
@@ -268,6 +268,30 @@
   </si>
   <si>
     <t>4.3</t>
+  </si>
+  <si>
+    <t>Criar menu principal</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Criar tabelas no banco de dados dos grupos</t>
+  </si>
+  <si>
+    <t>Criar endpoint para listar todos os grupos do usuário</t>
+  </si>
+  <si>
+    <t>Inserir na tela principal a lista de treinos do usuário</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t>12.3</t>
   </si>
 </sst>
 </file>
@@ -323,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -353,13 +377,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,10 +748,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -732,15 +759,15 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="5" t="s">
         <v>71</v>
       </c>
@@ -749,8 +776,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="5" t="s">
         <v>70</v>
       </c>
@@ -759,10 +786,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="11">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -773,8 +800,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
@@ -783,8 +810,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="6" t="s">
         <v>56</v>
       </c>
@@ -793,8 +820,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="5" t="s">
         <v>55</v>
       </c>
@@ -803,8 +830,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="5" t="s">
         <v>54</v>
       </c>
@@ -813,8 +840,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="5" t="s">
         <v>57</v>
       </c>
@@ -823,8 +850,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="5" t="s">
         <v>65</v>
       </c>
@@ -833,8 +860,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="5" t="s">
         <v>58</v>
       </c>
@@ -843,10 +870,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="A14" s="11">
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -855,24 +882,24 @@
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="7" t="s">
         <v>67</v>
       </c>
@@ -881,8 +908,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="1" t="s">
         <v>75</v>
       </c>
@@ -891,8 +918,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="8" t="s">
         <v>73</v>
       </c>
@@ -901,269 +928,309 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="11">
         <v>5</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="1" t="s">
+    <row r="22" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="1" t="s">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
         <v>6</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B24" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="1" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+    <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
         <v>7</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B28" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
         <v>8</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="1" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="1" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
         <v>9</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+    <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
         <v>10</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B34" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
         <v>11</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
+    <row r="37" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
         <v>12</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B37" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="1" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="1" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="1" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="1" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="1" t="s">
+    <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="1" t="s">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="1" t="s">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="5" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+    <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13">
         <v>13</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B49" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="5" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="13"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="5" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="5" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="5" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A36:A44"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B36:B44"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="B14:B19"/>
     <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A37:A48"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B37:B48"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-12.1 - CRUD grupos e grupos usuários
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E1D15-0586-414E-A874-6DD1D9FA5C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA3A7F2-5677-4E34-85E6-4B1F4843CFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -725,7 +725,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,10 +1140,10 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="10"/>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1160,10 +1160,10 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="10"/>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="5" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1217,6 +1217,8 @@
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="B14:B19"/>
     <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="A49:A52"/>
     <mergeCell ref="A37:A48"/>
@@ -1229,8 +1231,6 @@
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B37:B48"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-12.2 - Lista de grupos
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA3A7F2-5677-4E34-85E6-4B1F4843CFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70804378-6E8E-468D-A4EC-E310036955C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -725,7 +725,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,10 +1150,10 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="10"/>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="5" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GS-12.4 - Rotina de solicitações dos grupos de usuários
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70804378-6E8E-468D-A4EC-E310036955C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD144C24-3B2E-4478-98F3-BD364307A7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>User storys</t>
   </si>
@@ -292,6 +292,15 @@
   </si>
   <si>
     <t>12.3</t>
+  </si>
+  <si>
+    <t>Rotina de solicitações dos grupos</t>
+  </si>
+  <si>
+    <t>12.4</t>
+  </si>
+  <si>
+    <t>12.5</t>
   </si>
 </sst>
 </file>
@@ -347,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -374,6 +383,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -722,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,10 +760,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -759,15 +771,15 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="5" t="s">
         <v>71</v>
       </c>
@@ -776,8 +788,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="5" t="s">
         <v>70</v>
       </c>
@@ -786,10 +798,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="12">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -800,8 +812,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
@@ -810,8 +822,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="6" t="s">
         <v>56</v>
       </c>
@@ -820,8 +832,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="5" t="s">
         <v>55</v>
       </c>
@@ -830,8 +842,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="5" t="s">
         <v>54</v>
       </c>
@@ -840,8 +852,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="5" t="s">
         <v>57</v>
       </c>
@@ -850,8 +862,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="5" t="s">
         <v>65</v>
       </c>
@@ -860,8 +872,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="5" t="s">
         <v>58</v>
       </c>
@@ -870,10 +882,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="12">
         <v>4</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -882,24 +894,24 @@
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="7" t="s">
         <v>67</v>
       </c>
@@ -908,8 +920,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="1" t="s">
         <v>75</v>
       </c>
@@ -918,8 +930,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="8" t="s">
         <v>73</v>
       </c>
@@ -928,10 +940,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="A20" s="12">
         <v>5</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -942,31 +954,31 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="10"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="10"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="A24" s="12">
         <v>6</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -974,31 +986,31 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="10"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="10"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="A28" s="12">
         <v>7</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1006,17 +1018,17 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="10"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="A30" s="12">
         <v>8</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1024,15 +1036,15 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="10"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1049,10 +1061,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
+      <c r="A34" s="12">
         <v>10</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1060,8 +1072,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="10"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="1" t="s">
         <v>44</v>
       </c>
@@ -1077,135 +1089,148 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>12</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B38" s="11"/>
+      <c r="C38" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="1" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="1" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="1" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="1" t="s">
+    <row r="43" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="1" t="s">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="1" t="s">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="5" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D46" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="5" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="5" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="5" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13">
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
         <v>13</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B50" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="5" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="5" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="5" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1219,9 +1244,9 @@
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A37:A48"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A38:A49"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A32"/>
@@ -1230,7 +1255,7 @@
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B37:B48"/>
+    <mergeCell ref="B37:B49"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-12.5 - Rotina de ranking de grupos por quantidade de treinos realizados
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD144C24-3B2E-4478-98F3-BD364307A7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E02F207-217E-4E64-8AF6-0CDB13165891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
   <si>
     <t>User storys</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Criar telas para listar os grupos que usuário está dentro e detalhes do grupo como integrantes, treinos, frequencia dos outros usuários, ranking do grupo</t>
-  </si>
-  <si>
-    <t>Criar endpoint para retornar todos os detalhes do grupo</t>
   </si>
   <si>
     <t>notificações quando algum membro do meu grupo tiver feito um treino</t>
@@ -388,17 +385,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +747,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -760,10 +757,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -771,30 +768,30 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -805,10 +802,10 @@
         <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -818,67 +815,67 @@
         <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -913,63 +910,63 @@
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>5</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="B21" s="11"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
-      <c r="B22" s="11"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" s="11"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
@@ -978,7 +975,7 @@
       <c r="A24" s="12">
         <v>6</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -987,21 +984,21 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1010,7 +1007,7 @@
       <c r="A28" s="12">
         <v>7</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1019,7 +1016,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
-      <c r="B29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1028,7 +1025,7 @@
       <c r="A30" s="12">
         <v>8</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1037,16 +1034,16 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
-      <c r="B31" s="11"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
-      <c r="B32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1057,25 +1054,25 @@
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>10</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
-      <c r="B35" s="11"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1086,85 +1083,90 @@
         <v>8</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>12</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="13"/>
+      <c r="C38" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>87</v>
+      <c r="D38" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
-      <c r="B40" s="11"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="13"/>
+      <c r="C41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
-      <c r="B42" s="11"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
-      <c r="B43" s="11"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
-      <c r="B44" s="11"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="1" t="s">
-        <v>41</v>
+      <c r="B45" s="13"/>
+      <c r="C45" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
-      <c r="B46" s="11"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="5" t="s">
         <v>80</v>
       </c>
@@ -1174,9 +1176,9 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
-      <c r="B47" s="11"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>83</v>
@@ -1184,69 +1186,53 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
-      <c r="B48" s="11"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="11"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>13</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="C49" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14">
-        <v>13</v>
-      </c>
-      <c r="B50" s="13" t="s">
         <v>47</v>
       </c>
+      <c r="D49" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="14"/>
       <c r="C50" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="13"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="14"/>
       <c r="C51" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="A6:A13"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A14:A19"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A38:A48"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A32"/>
@@ -1255,7 +1241,13 @@
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B37:B49"/>
+    <mergeCell ref="B37:B48"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-12.6 - Publicações dentro dos grupos
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E02F207-217E-4E64-8AF6-0CDB13165891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91AB9F2-7F5E-458D-B2F8-CFDF8471A507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>User storys</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>12.5</t>
+  </si>
+  <si>
+    <t>12.6</t>
   </si>
 </sst>
 </file>
@@ -385,17 +388,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,10 +760,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -768,15 +771,15 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="5" t="s">
         <v>70</v>
       </c>
@@ -785,8 +788,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="5" t="s">
         <v>69</v>
       </c>
@@ -940,7 +943,7 @@
       <c r="A20" s="12">
         <v>5</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -952,21 +955,21 @@
     </row>
     <row r="21" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
@@ -975,7 +978,7 @@
       <c r="A24" s="12">
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -984,21 +987,21 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1007,7 +1010,7 @@
       <c r="A28" s="12">
         <v>7</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1016,7 +1019,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1025,7 +1028,7 @@
       <c r="A30" s="12">
         <v>8</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1034,14 +1037,14 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1061,7 +1064,7 @@
       <c r="A34" s="12">
         <v>10</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1070,7 +1073,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="1" t="s">
         <v>43</v>
       </c>
@@ -1088,7 +1091,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -1102,7 +1105,7 @@
       <c r="A38" s="12">
         <v>12</v>
       </c>
-      <c r="B38" s="13"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="5" t="s">
         <v>36</v>
       </c>
@@ -1112,7 +1115,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
-      <c r="B39" s="13"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="5" t="s">
         <v>33</v>
       </c>
@@ -1120,14 +1123,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="5" t="s">
         <v>35</v>
       </c>
@@ -1135,28 +1138,31 @@
     </row>
     <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
-      <c r="B42" s="13"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
-      <c r="B43" s="13"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D43" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
-      <c r="B44" s="13"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
-      <c r="B45" s="13"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="5" t="s">
         <v>79</v>
       </c>
@@ -1166,7 +1172,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
-      <c r="B46" s="13"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="5" t="s">
         <v>80</v>
       </c>
@@ -1176,7 +1182,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
-      <c r="B47" s="13"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="5" t="s">
         <v>78</v>
       </c>
@@ -1186,16 +1192,16 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
-      <c r="B48" s="13"/>
+      <c r="B48" s="11"/>
       <c r="C48" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+      <c r="A49" s="14">
         <v>13</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1206,28 +1212,34 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="14"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
-      <c r="B51" s="14"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="13"/>
       <c r="C51" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
-      <c r="B52" s="14"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="13"/>
       <c r="C52" s="5" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A14:A19"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="B49:B52"/>
@@ -1242,12 +1254,6 @@
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B37:B48"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="A6:A13"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-7.1 - Tela de calendário dos treinos executados + refresh token
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91AB9F2-7F5E-458D-B2F8-CFDF8471A507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9188289-D90A-48EC-8E62-390BEEB315CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
   <si>
     <t>User storys</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>12.6</t>
+  </si>
+  <si>
+    <t>7.1</t>
   </si>
 </sst>
 </file>
@@ -388,17 +391,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,10 +763,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -771,15 +774,15 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
         <v>70</v>
       </c>
@@ -788,8 +791,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="5" t="s">
         <v>69</v>
       </c>
@@ -943,7 +946,7 @@
       <c r="A20" s="12">
         <v>5</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -955,21 +958,21 @@
     </row>
     <row r="21" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="B21" s="11"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
-      <c r="B22" s="11"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" s="11"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
@@ -978,7 +981,7 @@
       <c r="A24" s="12">
         <v>6</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -987,21 +990,21 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1010,16 +1013,19 @@
       <c r="A28" s="12">
         <v>7</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="D28" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
-      <c r="B29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1028,7 +1034,7 @@
       <c r="A30" s="12">
         <v>8</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1037,14 +1043,14 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
-      <c r="B31" s="11"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
-      <c r="B32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1056,15 +1062,16 @@
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>10</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1073,7 +1080,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
-      <c r="B35" s="11"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="1" t="s">
         <v>43</v>
       </c>
@@ -1091,7 +1098,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -1105,7 +1112,7 @@
       <c r="A38" s="12">
         <v>12</v>
       </c>
-      <c r="B38" s="11"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="5" t="s">
         <v>36</v>
       </c>
@@ -1115,7 +1122,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
-      <c r="B39" s="11"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="5" t="s">
         <v>33</v>
       </c>
@@ -1123,14 +1130,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
-      <c r="B40" s="11"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
-      <c r="B41" s="11"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="5" t="s">
         <v>35</v>
       </c>
@@ -1138,31 +1145,32 @@
     </row>
     <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
-      <c r="B42" s="11"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="1" t="s">
+      <c r="B43" s="13"/>
+      <c r="C43" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="1" t="s">
+      <c r="B44" s="13"/>
+      <c r="C44" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
-      <c r="B45" s="11"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="5" t="s">
         <v>79</v>
       </c>
@@ -1172,7 +1180,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
-      <c r="B46" s="11"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="5" t="s">
         <v>80</v>
       </c>
@@ -1182,7 +1190,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
-      <c r="B47" s="11"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="5" t="s">
         <v>78</v>
       </c>
@@ -1192,54 +1200,49 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
-      <c r="B48" s="11"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14">
+      <c r="A49" s="11">
         <v>13</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="13"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="14"/>
       <c r="C50" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="13"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="14"/>
       <c r="C51" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="13"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="14"/>
       <c r="C52" s="5" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="A6:A13"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A14:A19"/>
+  <mergeCells count="21">
+    <mergeCell ref="D43:D44"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="B49:B52"/>
@@ -1254,6 +1257,12 @@
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B37:B48"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
GS-14.1 - Ajustes no Drawer, inclusão do email, nome e foto do usuário logado
</commit_message>
<xml_diff>
--- a/UserStorysTreinos.xlsx
+++ b/UserStorysTreinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppTreinos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9188289-D90A-48EC-8E62-390BEEB315CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51853FA1-1340-4BDC-BE22-B3413FFBD59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2ECFF8A6-4873-46D8-851B-0681A355078A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
   <si>
     <t>User storys</t>
   </si>
@@ -304,6 +304,33 @@
   </si>
   <si>
     <t>7.1</t>
+  </si>
+  <si>
+    <t>Eu como usuário quero ter acesso as configurações do aplicativo, personalizar imagem de perfil, etc</t>
+  </si>
+  <si>
+    <t>Criar tela de configuração para listar nome usuário, email, foto perfil</t>
+  </si>
+  <si>
+    <t>Criar rotina backend para retornar informações pessoais</t>
+  </si>
+  <si>
+    <t>Criar rotina backend para personalizar informações pessoais</t>
+  </si>
+  <si>
+    <t>Criar tela para edição de informações</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>Melhorar tela de ranking, mostra ordenado do maior para o menor</t>
+  </si>
+  <si>
+    <t>12.7</t>
   </si>
 </sst>
 </file>
@@ -359,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -391,17 +418,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6892303F-D306-4B83-A14F-73386835F189}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,10 +793,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -774,15 +804,15 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="5" t="s">
         <v>70</v>
       </c>
@@ -791,8 +821,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="5" t="s">
         <v>69</v>
       </c>
@@ -925,10 +955,10 @@
     <row r="18" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -946,7 +976,7 @@
       <c r="A20" s="12">
         <v>5</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -958,21 +988,23 @@
     </row>
     <row r="21" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
@@ -981,7 +1013,7 @@
       <c r="A24" s="12">
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -990,51 +1022,52 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12">
+      <c r="A28" s="13">
         <v>7</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="1" t="s">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>8</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1043,14 +1076,14 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1071,7 +1104,7 @@
       <c r="A34" s="12">
         <v>10</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1080,7 +1113,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="1" t="s">
         <v>43</v>
       </c>
@@ -1098,7 +1131,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -1112,7 +1145,7 @@
       <c r="A38" s="12">
         <v>12</v>
       </c>
-      <c r="B38" s="13"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="5" t="s">
         <v>36</v>
       </c>
@@ -1122,7 +1155,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
-      <c r="B39" s="13"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="5" t="s">
         <v>33</v>
       </c>
@@ -1130,14 +1163,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="5" t="s">
         <v>35</v>
       </c>
@@ -1145,109 +1178,158 @@
     </row>
     <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="11"/>
+      <c r="C42" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>87</v>
+      <c r="B43" s="11"/>
+      <c r="C43" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
-      <c r="B44" s="13"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="D45" s="13"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
-      <c r="B46" s="13"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
-      <c r="B47" s="13"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
-      <c r="B48" s="13"/>
+      <c r="B48" s="11"/>
       <c r="C48" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13">
         <v>13</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B50" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="14"/>
       <c r="C51" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
+      <c r="A52" s="13"/>
       <c r="B52" s="14"/>
       <c r="C52" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="5" t="s">
         <v>49</v>
       </c>
     </row>
+    <row r="54" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12">
+        <v>14</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="D43:D44"/>
+  <mergeCells count="23">
+    <mergeCell ref="D44:D45"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A38:A48"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A38:A49"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A32"/>
@@ -1256,7 +1338,9 @@
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B37:B48"/>
+    <mergeCell ref="B37:B49"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="A54:A57"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B6:B13"/>

</xml_diff>